<commit_message>
Yale dataset excel file update
</commit_message>
<xml_diff>
--- a/misc/Yaledataset+handover.xlsx
+++ b/misc/Yaledataset+handover.xlsx
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N76" sqref="N76"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +818,7 @@
     <col min="10" max="10" width="15.28515625" style="1"/>
     <col min="11" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="15.5703125" style="2"/>
-    <col min="14" max="14" width="15.140625" style="2"/>
+    <col min="14" max="14" width="19.85546875" style="2" customWidth="1"/>
     <col min="15" max="15" width="30.85546875" style="2"/>
     <col min="16" max="1025" width="9.140625" style="2"/>
   </cols>

</xml_diff>